<commit_message>
Addition of linear kernel for comparison & Gather results for different iterations and kernel functions
</commit_message>
<xml_diff>
--- a/yield_prediction/results/main_text_scores.xlsx
+++ b/yield_prediction/results/main_text_scores.xlsx
@@ -38,7 +38,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -78,6 +78,27 @@
       <left/>
       <right style="thin"/>
       <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -455,7 +476,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -582,55 +603,105 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>graph_descriptors</t>
+          <t>WLpolynomial_2</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>SVR - WL Kernel</t>
+          <t>SVR - Tanimoto Kernel</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.402</v>
+        <v>0.434</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6929999999999999</v>
+        <v>0.569</v>
       </c>
       <c r="F4" t="n">
-        <v>0.781</v>
+        <v>0.68</v>
       </c>
       <c r="G4" t="n">
-        <v>0.802</v>
+        <v>0.675</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6695</v>
+        <v>0.5894999999999999</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1844785443712448</v>
+        <v>0.1156157428726729</v>
       </c>
       <c r="J4" t="n">
-        <v>21.131</v>
+        <v>20.549</v>
       </c>
       <c r="K4" t="n">
-        <v>15.577</v>
+        <v>18.449</v>
       </c>
       <c r="L4" t="n">
-        <v>12.529</v>
+        <v>15.153</v>
       </c>
       <c r="M4" t="n">
-        <v>11.891</v>
+        <v>15.229</v>
       </c>
       <c r="N4" t="n">
-        <v>15.282</v>
+        <v>17.345</v>
       </c>
       <c r="O4" t="n">
-        <v>4.218045202855623</v>
+        <v>2.631017040360375</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n"/>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>WLpolynomial_3</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.397</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.6860000000000001</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.763</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.764</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.6525000000000001</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.1742077304063552</v>
+      </c>
+      <c r="J5" t="n">
+        <v>21.211</v>
+      </c>
+      <c r="K5" t="n">
+        <v>15.755</v>
+      </c>
+      <c r="L5" t="n">
+        <v>13.048</v>
+      </c>
+      <c r="M5" t="n">
+        <v>12.968</v>
+      </c>
+      <c r="N5" t="n">
+        <v>15.7455</v>
+      </c>
+      <c r="O5" t="n">
+        <v>3.867074389423266</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="J1:O1"/>
+    <mergeCell ref="A4:A5"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -642,7 +713,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -757,49 +828,93 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>graph_descriptors</t>
+          <t>WLpolynomial_2</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>SVR - WL Kernel</t>
+          <t>SVR - Tanimoto Kernel</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.59</v>
+        <v>0.652</v>
       </c>
       <c r="E4" t="n">
-        <v>0.696</v>
+        <v>0.652</v>
       </c>
       <c r="F4" t="n">
-        <v>0.539</v>
+        <v>0.673</v>
       </c>
       <c r="G4" t="n">
-        <v>0.6083333333333333</v>
+        <v>0.6590000000000001</v>
       </c>
       <c r="H4" t="n">
-        <v>0.08008953323208549</v>
+        <v>0.01212435565298215</v>
       </c>
       <c r="I4" t="n">
-        <v>15.953</v>
+        <v>14.693</v>
       </c>
       <c r="J4" t="n">
-        <v>14.685</v>
+        <v>15.707</v>
       </c>
       <c r="K4" t="n">
-        <v>17.986</v>
+        <v>15.16</v>
       </c>
       <c r="L4" t="n">
-        <v>16.208</v>
+        <v>15.18666666666667</v>
       </c>
       <c r="M4" t="n">
-        <v>1.665208395366778</v>
+        <v>0.5075256972147656</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n"/>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>WLpolynomial_3</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.654</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.661</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.658</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.6576666666666666</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.00351188458428425</v>
+      </c>
+      <c r="I5" t="n">
+        <v>14.646</v>
+      </c>
+      <c r="J5" t="n">
+        <v>15.516</v>
+      </c>
+      <c r="K5" t="n">
+        <v>15.488</v>
+      </c>
+      <c r="L5" t="n">
+        <v>15.21666666666667</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.4944100861970079</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="I1:M1"/>
+    <mergeCell ref="A4:A5"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Experiments: Linear & Poly (2 to 5 iterations)
</commit_message>
<xml_diff>
--- a/yield_prediction/results/main_text_scores.xlsx
+++ b/yield_prediction/results/main_text_scores.xlsx
@@ -476,7 +476,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -603,7 +603,7 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>WLpolynomial_2</t>
+          <t>WLlinear_2</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
@@ -612,96 +612,390 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.434</v>
+        <v>0.399</v>
       </c>
       <c r="E4" t="n">
-        <v>0.569</v>
+        <v>0.483</v>
       </c>
       <c r="F4" t="n">
-        <v>0.68</v>
+        <v>0.705</v>
       </c>
       <c r="G4" t="n">
-        <v>0.675</v>
+        <v>0.657</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5894999999999999</v>
+        <v>0.5609999999999999</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1156157428726729</v>
+        <v>0.144083309234623</v>
       </c>
       <c r="J4" t="n">
-        <v>20.549</v>
+        <v>21.182</v>
       </c>
       <c r="K4" t="n">
-        <v>18.449</v>
+        <v>20.192</v>
       </c>
       <c r="L4" t="n">
-        <v>15.153</v>
+        <v>14.543</v>
       </c>
       <c r="M4" t="n">
-        <v>15.229</v>
+        <v>15.642</v>
       </c>
       <c r="N4" t="n">
-        <v>17.345</v>
+        <v>17.88975</v>
       </c>
       <c r="O4" t="n">
-        <v>2.631017040360375</v>
+        <v>3.285948911653984</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
       <c r="B5" s="1" t="inlineStr">
         <is>
+          <t>WLlinear_3</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.434</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.569</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.5894999999999999</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.1156157428726729</v>
+      </c>
+      <c r="J5" t="n">
+        <v>20.549</v>
+      </c>
+      <c r="K5" t="n">
+        <v>18.449</v>
+      </c>
+      <c r="L5" t="n">
+        <v>15.153</v>
+      </c>
+      <c r="M5" t="n">
+        <v>15.229</v>
+      </c>
+      <c r="N5" t="n">
+        <v>17.345</v>
+      </c>
+      <c r="O5" t="n">
+        <v>2.631017040360375</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>WLlinear_4</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.397</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.6860000000000001</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.763</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.764</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.6525000000000001</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.1742077304063552</v>
+      </c>
+      <c r="J6" t="n">
+        <v>21.211</v>
+      </c>
+      <c r="K6" t="n">
+        <v>15.755</v>
+      </c>
+      <c r="L6" t="n">
+        <v>13.048</v>
+      </c>
+      <c r="M6" t="n">
+        <v>12.968</v>
+      </c>
+      <c r="N6" t="n">
+        <v>15.7455</v>
+      </c>
+      <c r="O6" t="n">
+        <v>3.867074389423266</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>WLlinear_5</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.408</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.6850000000000001</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.782</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.802</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.66925</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.1815073460405024</v>
+      </c>
+      <c r="J7" t="n">
+        <v>21.009</v>
+      </c>
+      <c r="K7" t="n">
+        <v>15.781</v>
+      </c>
+      <c r="L7" t="n">
+        <v>12.503</v>
+      </c>
+      <c r="M7" t="n">
+        <v>11.887</v>
+      </c>
+      <c r="N7" t="n">
+        <v>15.295</v>
+      </c>
+      <c r="O7" t="n">
+        <v>4.175153490192506</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>WLpolynomial_2</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>-6850913319.431</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-1013929984.927</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-931687733.544</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-1131547884.097</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-2482019730.49975</v>
+      </c>
+      <c r="I8" t="n">
+        <v>2913750286.782293</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2260961.023</v>
+      </c>
+      <c r="K8" t="n">
+        <v>894629.607</v>
+      </c>
+      <c r="L8" t="n">
+        <v>817374.3689999999</v>
+      </c>
+      <c r="M8" t="n">
+        <v>898473.429</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1217859.607</v>
+      </c>
+      <c r="O8" t="n">
+        <v>696403.6553404377</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
           <t>WLpolynomial_3</t>
         </is>
       </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>SVR - Tanimoto Kernel</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>0.397</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.6860000000000001</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.763</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.764</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.6525000000000001</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.1742077304063552</v>
-      </c>
-      <c r="J5" t="n">
-        <v>21.211</v>
-      </c>
-      <c r="K5" t="n">
-        <v>15.755</v>
-      </c>
-      <c r="L5" t="n">
-        <v>13.048</v>
-      </c>
-      <c r="M5" t="n">
-        <v>12.968</v>
-      </c>
-      <c r="N5" t="n">
-        <v>15.7455</v>
-      </c>
-      <c r="O5" t="n">
-        <v>3.867074389423266</v>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>-3256364943.523</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-1720042817.951</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-1579695069.37</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-2309081872.642</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-2216296175.8715</v>
+      </c>
+      <c r="I9" t="n">
+        <v>761988755.6072383</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1558781.973</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1165222.635</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1064320.574</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1283478.019</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1267950.80025</v>
+      </c>
+      <c r="O9" t="n">
+        <v>213574.5073298061</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>WLpolynomial_4</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>-6441337529.705</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-2561023699.095</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-2165858716.442</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-3527224563.25</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-3673861127.123</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1931571582.291854</v>
+      </c>
+      <c r="J10" t="n">
+        <v>2192334.75</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1421824.79</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1246237.708</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1586300.001</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1611674.31225</v>
+      </c>
+      <c r="O10" t="n">
+        <v>411257.0779385881</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n"/>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>WLpolynomial_5</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>-9143772361.903</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-3346823959.717</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-2815158532.523</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-4340203720.459</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-4911489643.650499</v>
+      </c>
+      <c r="I11" t="n">
+        <v>2891445281.240028</v>
+      </c>
+      <c r="J11" t="n">
+        <v>2612050.337</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1625383.018</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1420814.087</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1759640.004</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1854471.8615</v>
+      </c>
+      <c r="O11" t="n">
+        <v>523914.430461777</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="J1:O1"/>
-    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A4:A11"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -713,7 +1007,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -828,7 +1122,7 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>WLpolynomial_2</t>
+          <t>WLlinear_2</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
@@ -837,84 +1131,342 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.652</v>
+        <v>0.62</v>
       </c>
       <c r="E4" t="n">
-        <v>0.652</v>
+        <v>0.439</v>
       </c>
       <c r="F4" t="n">
-        <v>0.673</v>
+        <v>0.348</v>
       </c>
       <c r="G4" t="n">
-        <v>0.6590000000000001</v>
+        <v>0.469</v>
       </c>
       <c r="H4" t="n">
-        <v>0.01212435565298215</v>
+        <v>0.1384593803250614</v>
       </c>
       <c r="I4" t="n">
-        <v>14.693</v>
+        <v>15.349</v>
       </c>
       <c r="J4" t="n">
-        <v>15.707</v>
+        <v>19.955</v>
       </c>
       <c r="K4" t="n">
-        <v>15.16</v>
+        <v>21.389</v>
       </c>
       <c r="L4" t="n">
-        <v>15.18666666666667</v>
+        <v>18.89766666666667</v>
       </c>
       <c r="M4" t="n">
-        <v>0.5075256972147656</v>
+        <v>3.155766996046021</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
       <c r="B5" s="1" t="inlineStr">
         <is>
+          <t>WLlinear_3</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.652</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.652</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.673</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.6590000000000001</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.01212435565298215</v>
+      </c>
+      <c r="I5" t="n">
+        <v>14.693</v>
+      </c>
+      <c r="J5" t="n">
+        <v>15.707</v>
+      </c>
+      <c r="K5" t="n">
+        <v>15.16</v>
+      </c>
+      <c r="L5" t="n">
+        <v>15.18666666666667</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.5075256972147656</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>WLlinear_4</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.654</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.661</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.658</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.6576666666666666</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.00351188458428425</v>
+      </c>
+      <c r="I6" t="n">
+        <v>14.646</v>
+      </c>
+      <c r="J6" t="n">
+        <v>15.516</v>
+      </c>
+      <c r="K6" t="n">
+        <v>15.488</v>
+      </c>
+      <c r="L6" t="n">
+        <v>15.21666666666667</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.4944100861970079</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>WLlinear_5</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.707</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.614</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.6503333333333333</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.04972256362390551</v>
+      </c>
+      <c r="I7" t="n">
+        <v>15.162</v>
+      </c>
+      <c r="J7" t="n">
+        <v>14.427</v>
+      </c>
+      <c r="K7" t="n">
+        <v>16.453</v>
+      </c>
+      <c r="L7" t="n">
+        <v>15.34733333333333</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1.025636550310749</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>WLpolynomial_2</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>-4892818200.616</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-2887735226.785</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-2563297604.415</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-3447950343.938667</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1261763561.506984</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1742761.319</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1431608.864</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1341443.88</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1505271.354333333</v>
+      </c>
+      <c r="M8" t="n">
+        <v>210555.3218823048</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
           <t>WLpolynomial_3</t>
         </is>
       </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>SVR - Tanimoto Kernel</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>0.654</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.661</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.658</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.6576666666666666</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.00351188458428425</v>
-      </c>
-      <c r="I5" t="n">
-        <v>14.646</v>
-      </c>
-      <c r="J5" t="n">
-        <v>15.516</v>
-      </c>
-      <c r="K5" t="n">
-        <v>15.488</v>
-      </c>
-      <c r="L5" t="n">
-        <v>15.21666666666667</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.4944100861970079</v>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>-1824068284.429</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-3386993235.918</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-2598404734.782</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-2603155418.376334</v>
+      </c>
+      <c r="H9" t="n">
+        <v>781473305.8413984</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1064091.364</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1550432.48</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1350598.901</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1321707.581666667</v>
+      </c>
+      <c r="M9" t="n">
+        <v>244454.3955989477</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>WLpolynomial_4</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>-3399830827.72</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-2457728065.41</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-2274079752.97</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-2710546215.366666</v>
+      </c>
+      <c r="H10" t="n">
+        <v>603959132.1321573</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1452737.095</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1320725.636</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1263501.722</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1345654.817666667</v>
+      </c>
+      <c r="M10" t="n">
+        <v>97049.49599322774</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n"/>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>WLpolynomial_5</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>-4001389670.519</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-3106157096.922</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-2386855425.836</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-3164800731.092333</v>
+      </c>
+      <c r="H11" t="n">
+        <v>808863099.4705187</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1576027.517</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1484763.907</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1294452.294</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1451747.906</v>
+      </c>
+      <c r="M11" t="n">
+        <v>143661.7339217334</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="I1:M1"/>
-    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A4:A11"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Results with sigmoid functions
</commit_message>
<xml_diff>
--- a/yield_prediction/results/main_text_scores.xlsx
+++ b/yield_prediction/results/main_text_scores.xlsx
@@ -476,7 +476,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -750,7 +750,7 @@
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>WLpolynomial_2</t>
+          <t>WLlinear_5</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
@@ -759,47 +759,47 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.433</v>
+        <v>0.408</v>
       </c>
       <c r="E7" t="n">
-        <v>0.222</v>
+        <v>0.6850000000000001</v>
       </c>
       <c r="F7" t="n">
-        <v>0.743</v>
+        <v>0.782</v>
       </c>
       <c r="G7" t="n">
-        <v>0.595</v>
+        <v>0.802</v>
       </c>
       <c r="H7" t="n">
-        <v>0.49825</v>
+        <v>0.66925</v>
       </c>
       <c r="I7" t="n">
-        <v>0.2234835937304273</v>
+        <v>0.1815073460405024</v>
       </c>
       <c r="J7" t="n">
-        <v>20.567</v>
+        <v>21.009</v>
       </c>
       <c r="K7" t="n">
-        <v>24.774</v>
+        <v>15.781</v>
       </c>
       <c r="L7" t="n">
-        <v>13.587</v>
+        <v>12.503</v>
       </c>
       <c r="M7" t="n">
-        <v>16.995</v>
+        <v>11.887</v>
       </c>
       <c r="N7" t="n">
-        <v>18.98075</v>
+        <v>15.295</v>
       </c>
       <c r="O7" t="n">
-        <v>4.799780437686708</v>
+        <v>4.175153490192506</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>WLpolynomial_3</t>
+          <t>WLpolynomial_2</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
@@ -808,96 +808,782 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.446</v>
+        <v>0.433</v>
       </c>
       <c r="E8" t="n">
-        <v>0.665</v>
+        <v>0.222</v>
       </c>
       <c r="F8" t="n">
-        <v>0.724</v>
+        <v>0.743</v>
       </c>
       <c r="G8" t="n">
-        <v>0.732</v>
+        <v>0.595</v>
       </c>
       <c r="H8" t="n">
-        <v>0.64175</v>
+        <v>0.49825</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1338764978129719</v>
+        <v>0.2234835937304273</v>
       </c>
       <c r="J8" t="n">
-        <v>20.332</v>
+        <v>20.567</v>
       </c>
       <c r="K8" t="n">
-        <v>16.254</v>
+        <v>24.774</v>
       </c>
       <c r="L8" t="n">
-        <v>14.07</v>
+        <v>13.587</v>
       </c>
       <c r="M8" t="n">
-        <v>13.83</v>
+        <v>16.995</v>
       </c>
       <c r="N8" t="n">
-        <v>16.1215</v>
+        <v>18.98075</v>
       </c>
       <c r="O8" t="n">
-        <v>3.011394527457337</v>
+        <v>4.799780437686708</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
+          <t>WLpolynomial_3</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.446</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.665</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.724</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.732</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.64175</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.1338764978129719</v>
+      </c>
+      <c r="J9" t="n">
+        <v>20.332</v>
+      </c>
+      <c r="K9" t="n">
+        <v>16.254</v>
+      </c>
+      <c r="L9" t="n">
+        <v>14.07</v>
+      </c>
+      <c r="M9" t="n">
+        <v>13.83</v>
+      </c>
+      <c r="N9" t="n">
+        <v>16.1215</v>
+      </c>
+      <c r="O9" t="n">
+        <v>3.011394527457337</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
           <t>WLpolynomial_4</t>
         </is>
       </c>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t>SVR - Tanimoto Kernel</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
         <v>0.4</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E10" t="n">
         <v>0.6919999999999999</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F10" t="n">
         <v>0.781</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G10" t="n">
         <v>0.786</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H10" t="n">
         <v>0.6647500000000001</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I10" t="n">
         <v>0.1817055768727715</v>
       </c>
-      <c r="J9" t="n">
+      <c r="J10" t="n">
         <v>21.161</v>
       </c>
-      <c r="K9" t="n">
+      <c r="K10" t="n">
         <v>15.603</v>
       </c>
-      <c r="L9" t="n">
+      <c r="L10" t="n">
         <v>12.527</v>
       </c>
-      <c r="M9" t="n">
+      <c r="M10" t="n">
         <v>12.357</v>
       </c>
-      <c r="N9" t="n">
+      <c r="N10" t="n">
         <v>15.412</v>
       </c>
-      <c r="O9" t="n">
+      <c r="O10" t="n">
         <v>4.112733559730479</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n"/>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>WLpolynomial_5</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.408</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.665</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.766</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.8080000000000001</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.6617500000000001</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.1794962859411489</v>
+      </c>
+      <c r="J11" t="n">
+        <v>21.019</v>
+      </c>
+      <c r="K11" t="n">
+        <v>16.263</v>
+      </c>
+      <c r="L11" t="n">
+        <v>12.945</v>
+      </c>
+      <c r="M11" t="n">
+        <v>11.709</v>
+      </c>
+      <c r="N11" t="n">
+        <v>15.484</v>
+      </c>
+      <c r="O11" t="n">
+        <v>4.160937875046922</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n"/>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidarctangent_2</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>-4.555</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-1.957</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-2.049</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-1.106</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-2.41675</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1.48736778123861</v>
+      </c>
+      <c r="J12" t="n">
+        <v>64.38200000000001</v>
+      </c>
+      <c r="K12" t="n">
+        <v>48.309</v>
+      </c>
+      <c r="L12" t="n">
+        <v>46.76</v>
+      </c>
+      <c r="M12" t="n">
+        <v>38.762</v>
+      </c>
+      <c r="N12" t="n">
+        <v>49.55325</v>
+      </c>
+      <c r="O12" t="n">
+        <v>10.73457508474369</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n"/>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidarctangent_3</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.594</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-0.627</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-0.5610000000000001</v>
+      </c>
+      <c r="G13" t="n">
+        <v>-0.137</v>
+      </c>
+      <c r="H13" t="n">
+        <v>-0.47975</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.2300831371482925</v>
+      </c>
+      <c r="J13" t="n">
+        <v>34.49</v>
+      </c>
+      <c r="K13" t="n">
+        <v>35.835</v>
+      </c>
+      <c r="L13" t="n">
+        <v>33.459</v>
+      </c>
+      <c r="M13" t="n">
+        <v>28.485</v>
+      </c>
+      <c r="N13" t="n">
+        <v>33.06725</v>
+      </c>
+      <c r="O13" t="n">
+        <v>3.205991305353152</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n"/>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidarctangent_4</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>-0.134</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-0.127</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="H14" t="n">
+        <v>-0.02950000000000001</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.1304517790858625</v>
+      </c>
+      <c r="J14" t="n">
+        <v>29.087</v>
+      </c>
+      <c r="K14" t="n">
+        <v>29.831</v>
+      </c>
+      <c r="L14" t="n">
+        <v>26.773</v>
+      </c>
+      <c r="M14" t="n">
+        <v>24.732</v>
+      </c>
+      <c r="N14" t="n">
+        <v>27.60575</v>
+      </c>
+      <c r="O14" t="n">
+        <v>2.316444887465848</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n"/>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidarctangent_5</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.273</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.279</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.16675</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.1376865401313191</v>
+      </c>
+      <c r="J15" t="n">
+        <v>25.557</v>
+      </c>
+      <c r="K15" t="n">
+        <v>23.964</v>
+      </c>
+      <c r="L15" t="n">
+        <v>26.911</v>
+      </c>
+      <c r="M15" t="n">
+        <v>22.686</v>
+      </c>
+      <c r="N15" t="n">
+        <v>24.7795</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1.843509424982688</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n"/>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_2</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.251</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.433</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.468</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.448</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.1003626756651429</v>
+      </c>
+      <c r="J16" t="n">
+        <v>23.639</v>
+      </c>
+      <c r="K16" t="n">
+        <v>21.153</v>
+      </c>
+      <c r="L16" t="n">
+        <v>19.53</v>
+      </c>
+      <c r="M16" t="n">
+        <v>19.839</v>
+      </c>
+      <c r="N16" t="n">
+        <v>21.04025</v>
+      </c>
+      <c r="O16" t="n">
+        <v>1.869943916271287</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n"/>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_3</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.354</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.509</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.541</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.545</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.48725</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.09028242723070018</v>
+      </c>
+      <c r="J17" t="n">
+        <v>21.952</v>
+      </c>
+      <c r="K17" t="n">
+        <v>19.691</v>
+      </c>
+      <c r="L17" t="n">
+        <v>18.141</v>
+      </c>
+      <c r="M17" t="n">
+        <v>18.015</v>
+      </c>
+      <c r="N17" t="n">
+        <v>19.44975</v>
+      </c>
+      <c r="O17" t="n">
+        <v>1.83401115500061</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n"/>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_4</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.367</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.5580000000000001</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.49725</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.087937003966855</v>
+      </c>
+      <c r="J18" t="n">
+        <v>21.725</v>
+      </c>
+      <c r="K18" t="n">
+        <v>19.38</v>
+      </c>
+      <c r="L18" t="n">
+        <v>18.162</v>
+      </c>
+      <c r="M18" t="n">
+        <v>17.752</v>
+      </c>
+      <c r="N18" t="n">
+        <v>19.25475</v>
+      </c>
+      <c r="O18" t="n">
+        <v>1.786074163260493</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n"/>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_5</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.202</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.391</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.456</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.495</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.386</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.1299512729192497</v>
+      </c>
+      <c r="J19" t="n">
+        <v>24.4</v>
+      </c>
+      <c r="K19" t="n">
+        <v>21.925</v>
+      </c>
+      <c r="L19" t="n">
+        <v>19.754</v>
+      </c>
+      <c r="M19" t="n">
+        <v>18.979</v>
+      </c>
+      <c r="N19" t="n">
+        <v>21.2645</v>
+      </c>
+      <c r="O19" t="n">
+        <v>2.433977608771288</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n"/>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidlogistic_2</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.115</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.188</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.245</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.189</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.18425</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.05330025015576068</v>
+      </c>
+      <c r="J20" t="n">
+        <v>25.702</v>
+      </c>
+      <c r="K20" t="n">
+        <v>25.325</v>
+      </c>
+      <c r="L20" t="n">
+        <v>23.269</v>
+      </c>
+      <c r="M20" t="n">
+        <v>24.049</v>
+      </c>
+      <c r="N20" t="n">
+        <v>24.58625</v>
+      </c>
+      <c r="O20" t="n">
+        <v>1.127598443595947</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n"/>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidlogistic_3</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.207</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.295</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.363</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.313</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.2945</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.06504101270224298</v>
+      </c>
+      <c r="J21" t="n">
+        <v>24.326</v>
+      </c>
+      <c r="K21" t="n">
+        <v>23.585</v>
+      </c>
+      <c r="L21" t="n">
+        <v>21.378</v>
+      </c>
+      <c r="M21" t="n">
+        <v>22.133</v>
+      </c>
+      <c r="N21" t="n">
+        <v>22.8555</v>
+      </c>
+      <c r="O21" t="n">
+        <v>1.341585256329243</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n"/>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidlogistic_4</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.242</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.342</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.397</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.358</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.33475</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.06600694407913964</v>
+      </c>
+      <c r="J22" t="n">
+        <v>23.782</v>
+      </c>
+      <c r="K22" t="n">
+        <v>22.789</v>
+      </c>
+      <c r="L22" t="n">
+        <v>20.789</v>
+      </c>
+      <c r="M22" t="n">
+        <v>21.394</v>
+      </c>
+      <c r="N22" t="n">
+        <v>22.1885</v>
+      </c>
+      <c r="O22" t="n">
+        <v>1.352734637687673</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n"/>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidlogistic_5</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.271</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.365</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.422</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.382</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.06396353127629315</v>
+      </c>
+      <c r="J23" t="n">
+        <v>23.326</v>
+      </c>
+      <c r="K23" t="n">
+        <v>22.386</v>
+      </c>
+      <c r="L23" t="n">
+        <v>20.355</v>
+      </c>
+      <c r="M23" t="n">
+        <v>20.996</v>
+      </c>
+      <c r="N23" t="n">
+        <v>21.76575</v>
+      </c>
+      <c r="O23" t="n">
+        <v>1.341866951924321</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="J1:O1"/>
-    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="A4:A23"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -909,7 +1595,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1153,7 +1839,7 @@
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>WLpolynomial_2</t>
+          <t>WLlinear_5</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
@@ -1162,41 +1848,41 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.656</v>
+        <v>0.63</v>
       </c>
       <c r="E7" t="n">
-        <v>0.434</v>
+        <v>0.707</v>
       </c>
       <c r="F7" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.614</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3923333333333334</v>
+        <v>0.6503333333333333</v>
       </c>
       <c r="H7" t="n">
-        <v>0.2867792414616744</v>
+        <v>0.04972256362390551</v>
       </c>
       <c r="I7" t="n">
-        <v>14.605</v>
+        <v>15.162</v>
       </c>
       <c r="J7" t="n">
-        <v>20.039</v>
+        <v>14.427</v>
       </c>
       <c r="K7" t="n">
-        <v>25.317</v>
+        <v>16.453</v>
       </c>
       <c r="L7" t="n">
-        <v>19.987</v>
+        <v>15.34733333333333</v>
       </c>
       <c r="M7" t="n">
-        <v>5.356189317042481</v>
+        <v>1.025636550310749</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>WLpolynomial_3</t>
+          <t>WLpolynomial_2</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
@@ -1205,84 +1891,686 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.652</v>
+        <v>0.656</v>
       </c>
       <c r="E8" t="n">
-        <v>0.6840000000000001</v>
+        <v>0.434</v>
       </c>
       <c r="F8" t="n">
-        <v>0.655</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="G8" t="n">
-        <v>0.6636666666666667</v>
+        <v>0.3923333333333334</v>
       </c>
       <c r="H8" t="n">
-        <v>0.01767295485574876</v>
+        <v>0.2867792414616744</v>
       </c>
       <c r="I8" t="n">
-        <v>14.708</v>
+        <v>14.605</v>
       </c>
       <c r="J8" t="n">
-        <v>14.98</v>
+        <v>20.039</v>
       </c>
       <c r="K8" t="n">
-        <v>15.554</v>
+        <v>25.317</v>
       </c>
       <c r="L8" t="n">
-        <v>15.08066666666667</v>
+        <v>19.987</v>
       </c>
       <c r="M8" t="n">
-        <v>0.4318904182004196</v>
+        <v>5.356189317042481</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
+          <t>WLpolynomial_3</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.652</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.6840000000000001</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.655</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.6636666666666667</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.01767295485574876</v>
+      </c>
+      <c r="I9" t="n">
+        <v>14.708</v>
+      </c>
+      <c r="J9" t="n">
+        <v>14.98</v>
+      </c>
+      <c r="K9" t="n">
+        <v>15.554</v>
+      </c>
+      <c r="L9" t="n">
+        <v>15.08066666666667</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.4318904182004196</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
           <t>WLpolynomial_4</t>
         </is>
       </c>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t>SVR - Tanimoto Kernel</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
         <v>0.653</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E10" t="n">
         <v>0.667</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F10" t="n">
         <v>0.638</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G10" t="n">
         <v>0.6526666666666667</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H10" t="n">
         <v>0.01450287327853807</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I10" t="n">
         <v>14.684</v>
       </c>
-      <c r="J9" t="n">
+      <c r="J10" t="n">
         <v>15.373</v>
       </c>
-      <c r="K9" t="n">
+      <c r="K10" t="n">
         <v>15.932</v>
       </c>
-      <c r="L9" t="n">
+      <c r="L10" t="n">
         <v>15.32966666666667</v>
       </c>
-      <c r="M9" t="n">
+      <c r="M10" t="n">
         <v>0.6251274536711166</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n"/>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>WLpolynomial_5</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.656</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.579</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.6083333333333333</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.04164532786920205</v>
+      </c>
+      <c r="I11" t="n">
+        <v>15.945</v>
+      </c>
+      <c r="J11" t="n">
+        <v>15.623</v>
+      </c>
+      <c r="K11" t="n">
+        <v>17.187</v>
+      </c>
+      <c r="L11" t="n">
+        <v>16.25166666666667</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.8258676245823751</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n"/>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidarctangent_2</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>-2.025</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-2.106</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-2.23</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-2.120333333333333</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.1032488902280956</v>
+      </c>
+      <c r="I12" t="n">
+        <v>43.335</v>
+      </c>
+      <c r="J12" t="n">
+        <v>46.953</v>
+      </c>
+      <c r="K12" t="n">
+        <v>47.615</v>
+      </c>
+      <c r="L12" t="n">
+        <v>45.96766666666667</v>
+      </c>
+      <c r="M12" t="n">
+        <v>2.30385792386018</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n"/>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidarctangent_3</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.14</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-0.347</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-0.291</v>
+      </c>
+      <c r="G13" t="n">
+        <v>-0.2593333333333333</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.1070716271163063</v>
+      </c>
+      <c r="I13" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="J13" t="n">
+        <v>30.916</v>
+      </c>
+      <c r="K13" t="n">
+        <v>30.109</v>
+      </c>
+      <c r="L13" t="n">
+        <v>29.20833333333333</v>
+      </c>
+      <c r="M13" t="n">
+        <v>2.294638170460287</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n"/>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidarctangent_4</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>-0.099</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.176</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.109</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.1838939912014528</v>
+      </c>
+      <c r="I14" t="n">
+        <v>26.125</v>
+      </c>
+      <c r="J14" t="n">
+        <v>23.071</v>
+      </c>
+      <c r="K14" t="n">
+        <v>24.053</v>
+      </c>
+      <c r="L14" t="n">
+        <v>24.41633333333333</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1.559082208651401</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n"/>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidarctangent_5</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.142</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.1123333333333333</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.07129048557369583</v>
+      </c>
+      <c r="I15" t="n">
+        <v>22.778</v>
+      </c>
+      <c r="J15" t="n">
+        <v>24.679</v>
+      </c>
+      <c r="K15" t="n">
+        <v>26.076</v>
+      </c>
+      <c r="L15" t="n">
+        <v>24.511</v>
+      </c>
+      <c r="M15" t="n">
+        <v>1.655405992498518</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n"/>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_2</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.334</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.468</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.249</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.3503333333333334</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.1104098425564195</v>
+      </c>
+      <c r="I16" t="n">
+        <v>20.325</v>
+      </c>
+      <c r="J16" t="n">
+        <v>19.435</v>
+      </c>
+      <c r="K16" t="n">
+        <v>22.962</v>
+      </c>
+      <c r="L16" t="n">
+        <v>20.90733333333333</v>
+      </c>
+      <c r="M16" t="n">
+        <v>1.834193646628767</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n"/>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_3</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.522</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.381</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.4476666666666667</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.07081195755896977</v>
+      </c>
+      <c r="I17" t="n">
+        <v>18.643</v>
+      </c>
+      <c r="J17" t="n">
+        <v>18.428</v>
+      </c>
+      <c r="K17" t="n">
+        <v>20.841</v>
+      </c>
+      <c r="L17" t="n">
+        <v>19.304</v>
+      </c>
+      <c r="M17" t="n">
+        <v>1.335414916795526</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n"/>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_4</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.421</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.486</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.357</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.4213333333333333</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.06450064599159712</v>
+      </c>
+      <c r="I18" t="n">
+        <v>18.955</v>
+      </c>
+      <c r="J18" t="n">
+        <v>19.091</v>
+      </c>
+      <c r="K18" t="n">
+        <v>21.254</v>
+      </c>
+      <c r="L18" t="n">
+        <v>19.76666666666667</v>
+      </c>
+      <c r="M18" t="n">
+        <v>1.289862137336133</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n"/>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_5</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.509</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.416</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.304</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.4096666666666667</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.1026466430689934</v>
+      </c>
+      <c r="I19" t="n">
+        <v>17.461</v>
+      </c>
+      <c r="J19" t="n">
+        <v>20.361</v>
+      </c>
+      <c r="K19" t="n">
+        <v>22.098</v>
+      </c>
+      <c r="L19" t="n">
+        <v>19.97333333333333</v>
+      </c>
+      <c r="M19" t="n">
+        <v>2.342681440856468</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n"/>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidlogistic_2</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.097</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.227</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.06900000000000001</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.131</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.08430895563343198</v>
+      </c>
+      <c r="I20" t="n">
+        <v>23.681</v>
+      </c>
+      <c r="J20" t="n">
+        <v>23.429</v>
+      </c>
+      <c r="K20" t="n">
+        <v>25.572</v>
+      </c>
+      <c r="L20" t="n">
+        <v>24.22733333333333</v>
+      </c>
+      <c r="M20" t="n">
+        <v>1.171312227091194</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n"/>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidlogistic_3</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.213</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.299</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.158</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.2233333333333333</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.07106569730420811</v>
+      </c>
+      <c r="I21" t="n">
+        <v>22.102</v>
+      </c>
+      <c r="J21" t="n">
+        <v>22.312</v>
+      </c>
+      <c r="K21" t="n">
+        <v>24.309</v>
+      </c>
+      <c r="L21" t="n">
+        <v>22.90766666666667</v>
+      </c>
+      <c r="M21" t="n">
+        <v>1.218124104241162</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n"/>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidlogistic_4</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.245</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.303</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.168</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.2386666666666667</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.06772247288259144</v>
+      </c>
+      <c r="I22" t="n">
+        <v>21.654</v>
+      </c>
+      <c r="J22" t="n">
+        <v>22.235</v>
+      </c>
+      <c r="K22" t="n">
+        <v>24.172</v>
+      </c>
+      <c r="L22" t="n">
+        <v>22.687</v>
+      </c>
+      <c r="M22" t="n">
+        <v>1.318449468125344</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n"/>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidlogistic_5</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.249</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.305</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.178</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.244</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.06364746656387826</v>
+      </c>
+      <c r="I23" t="n">
+        <v>21.586</v>
+      </c>
+      <c r="J23" t="n">
+        <v>22.217</v>
+      </c>
+      <c r="K23" t="n">
+        <v>24.02</v>
+      </c>
+      <c r="L23" t="n">
+        <v>22.60766666666666</v>
+      </c>
+      <c r="M23" t="n">
+        <v>1.26315253763484</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="I1:M1"/>
-    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="A4:A23"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Results: linear; poly; sigmoid; rbf
</commit_message>
<xml_diff>
--- a/yield_prediction/results/main_text_scores.xlsx
+++ b/yield_prediction/results/main_text_scores.xlsx
@@ -476,7 +476,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -603,7 +603,7 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>WLlinear_2</t>
+          <t>WLlinear_10</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
@@ -612,47 +612,47 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.399</v>
+        <v>0.491</v>
       </c>
       <c r="E4" t="n">
-        <v>0.483</v>
+        <v>0.654</v>
       </c>
       <c r="F4" t="n">
-        <v>0.705</v>
+        <v>0.751</v>
       </c>
       <c r="G4" t="n">
-        <v>0.657</v>
+        <v>0.788</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5609999999999999</v>
+        <v>0.671</v>
       </c>
       <c r="I4" t="n">
-        <v>0.144083309234623</v>
+        <v>0.1326373501946818</v>
       </c>
       <c r="J4" t="n">
-        <v>21.182</v>
+        <v>19.481</v>
       </c>
       <c r="K4" t="n">
-        <v>20.192</v>
+        <v>16.522</v>
       </c>
       <c r="L4" t="n">
-        <v>14.543</v>
+        <v>13.363</v>
       </c>
       <c r="M4" t="n">
-        <v>15.642</v>
+        <v>12.292</v>
       </c>
       <c r="N4" t="n">
-        <v>17.88975</v>
+        <v>15.4145</v>
       </c>
       <c r="O4" t="n">
-        <v>3.285948911653984</v>
+        <v>3.251750144153146</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>WLlinear_3</t>
+          <t>WLlinear_2</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
@@ -661,47 +661,47 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.434</v>
+        <v>0.399</v>
       </c>
       <c r="E5" t="n">
-        <v>0.569</v>
+        <v>0.483</v>
       </c>
       <c r="F5" t="n">
-        <v>0.68</v>
+        <v>0.705</v>
       </c>
       <c r="G5" t="n">
-        <v>0.675</v>
+        <v>0.657</v>
       </c>
       <c r="H5" t="n">
-        <v>0.5894999999999999</v>
+        <v>0.5609999999999999</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1156157428726729</v>
+        <v>0.144083309234623</v>
       </c>
       <c r="J5" t="n">
-        <v>20.549</v>
+        <v>21.182</v>
       </c>
       <c r="K5" t="n">
-        <v>18.449</v>
+        <v>20.192</v>
       </c>
       <c r="L5" t="n">
-        <v>15.153</v>
+        <v>14.543</v>
       </c>
       <c r="M5" t="n">
-        <v>15.229</v>
+        <v>15.642</v>
       </c>
       <c r="N5" t="n">
-        <v>17.345</v>
+        <v>17.88975</v>
       </c>
       <c r="O5" t="n">
-        <v>2.631017040360375</v>
+        <v>3.285948911653984</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>WLlinear_4</t>
+          <t>WLlinear_3</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
@@ -710,47 +710,47 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.397</v>
+        <v>0.434</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6860000000000001</v>
+        <v>0.569</v>
       </c>
       <c r="F6" t="n">
-        <v>0.763</v>
+        <v>0.68</v>
       </c>
       <c r="G6" t="n">
-        <v>0.764</v>
+        <v>0.675</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6525000000000001</v>
+        <v>0.5894999999999999</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1742077304063552</v>
+        <v>0.1156157428726729</v>
       </c>
       <c r="J6" t="n">
-        <v>21.211</v>
+        <v>20.549</v>
       </c>
       <c r="K6" t="n">
-        <v>15.755</v>
+        <v>18.449</v>
       </c>
       <c r="L6" t="n">
-        <v>13.048</v>
+        <v>15.153</v>
       </c>
       <c r="M6" t="n">
-        <v>12.968</v>
+        <v>15.229</v>
       </c>
       <c r="N6" t="n">
-        <v>15.7455</v>
+        <v>17.345</v>
       </c>
       <c r="O6" t="n">
-        <v>3.867074389423266</v>
+        <v>2.631017040360375</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>WLlinear_5</t>
+          <t>WLlinear_4</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
@@ -759,47 +759,47 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.408</v>
+        <v>0.397</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6850000000000001</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="F7" t="n">
-        <v>0.782</v>
+        <v>0.763</v>
       </c>
       <c r="G7" t="n">
-        <v>0.802</v>
+        <v>0.764</v>
       </c>
       <c r="H7" t="n">
-        <v>0.66925</v>
+        <v>0.6525000000000001</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1815073460405024</v>
+        <v>0.1742077304063552</v>
       </c>
       <c r="J7" t="n">
-        <v>21.009</v>
+        <v>21.211</v>
       </c>
       <c r="K7" t="n">
-        <v>15.781</v>
+        <v>15.755</v>
       </c>
       <c r="L7" t="n">
-        <v>12.503</v>
+        <v>13.048</v>
       </c>
       <c r="M7" t="n">
-        <v>11.887</v>
+        <v>12.968</v>
       </c>
       <c r="N7" t="n">
-        <v>15.295</v>
+        <v>15.7455</v>
       </c>
       <c r="O7" t="n">
-        <v>4.175153490192506</v>
+        <v>3.867074389423266</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>WLpolynomial_2</t>
+          <t>WLlinear_5</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
@@ -808,47 +808,47 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.433</v>
+        <v>0.408</v>
       </c>
       <c r="E8" t="n">
-        <v>0.222</v>
+        <v>0.6850000000000001</v>
       </c>
       <c r="F8" t="n">
-        <v>0.743</v>
+        <v>0.782</v>
       </c>
       <c r="G8" t="n">
-        <v>0.595</v>
+        <v>0.802</v>
       </c>
       <c r="H8" t="n">
-        <v>0.49825</v>
+        <v>0.66925</v>
       </c>
       <c r="I8" t="n">
-        <v>0.2234835937304273</v>
+        <v>0.1815073460405024</v>
       </c>
       <c r="J8" t="n">
-        <v>20.567</v>
+        <v>21.009</v>
       </c>
       <c r="K8" t="n">
-        <v>24.774</v>
+        <v>15.781</v>
       </c>
       <c r="L8" t="n">
-        <v>13.587</v>
+        <v>12.503</v>
       </c>
       <c r="M8" t="n">
-        <v>16.995</v>
+        <v>11.887</v>
       </c>
       <c r="N8" t="n">
-        <v>18.98075</v>
+        <v>15.295</v>
       </c>
       <c r="O8" t="n">
-        <v>4.799780437686708</v>
+        <v>4.175153490192506</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>WLpolynomial_3</t>
+          <t>WLlinear_6</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr">
@@ -857,47 +857,47 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.446</v>
+        <v>0.42</v>
       </c>
       <c r="E9" t="n">
-        <v>0.665</v>
+        <v>0.679</v>
       </c>
       <c r="F9" t="n">
-        <v>0.724</v>
+        <v>0.775</v>
       </c>
       <c r="G9" t="n">
-        <v>0.732</v>
+        <v>0.8080000000000001</v>
       </c>
       <c r="H9" t="n">
-        <v>0.64175</v>
+        <v>0.6705000000000001</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1338764978129719</v>
+        <v>0.1757355968493578</v>
       </c>
       <c r="J9" t="n">
-        <v>20.332</v>
+        <v>20.804</v>
       </c>
       <c r="K9" t="n">
-        <v>16.254</v>
+        <v>15.927</v>
       </c>
       <c r="L9" t="n">
-        <v>14.07</v>
+        <v>12.689</v>
       </c>
       <c r="M9" t="n">
-        <v>13.83</v>
+        <v>11.689</v>
       </c>
       <c r="N9" t="n">
-        <v>16.1215</v>
+        <v>15.27725</v>
       </c>
       <c r="O9" t="n">
-        <v>3.011394527457337</v>
+        <v>4.10453881899863</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>WLpolynomial_4</t>
+          <t>WLlinear_7</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr">
@@ -906,47 +906,47 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.4</v>
+        <v>0.444</v>
       </c>
       <c r="E10" t="n">
-        <v>0.6919999999999999</v>
+        <v>0.672</v>
       </c>
       <c r="F10" t="n">
-        <v>0.781</v>
+        <v>0.765</v>
       </c>
       <c r="G10" t="n">
-        <v>0.786</v>
+        <v>0.8090000000000001</v>
       </c>
       <c r="H10" t="n">
-        <v>0.6647500000000001</v>
+        <v>0.6725000000000001</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1817055768727715</v>
+        <v>0.1626868156919915</v>
       </c>
       <c r="J10" t="n">
-        <v>21.161</v>
+        <v>20.369</v>
       </c>
       <c r="K10" t="n">
-        <v>15.603</v>
+        <v>16.102</v>
       </c>
       <c r="L10" t="n">
-        <v>12.527</v>
+        <v>12.993</v>
       </c>
       <c r="M10" t="n">
-        <v>12.357</v>
+        <v>11.673</v>
       </c>
       <c r="N10" t="n">
-        <v>15.412</v>
+        <v>15.28425</v>
       </c>
       <c r="O10" t="n">
-        <v>4.112733559730479</v>
+        <v>3.864986017654743</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>WLpolynomial_5</t>
+          <t>WLlinear_8</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr">
@@ -955,47 +955,47 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.408</v>
+        <v>0.464</v>
       </c>
       <c r="E11" t="n">
         <v>0.665</v>
       </c>
       <c r="F11" t="n">
-        <v>0.766</v>
+        <v>0.757</v>
       </c>
       <c r="G11" t="n">
-        <v>0.8080000000000001</v>
+        <v>0.802</v>
       </c>
       <c r="H11" t="n">
-        <v>0.6617500000000001</v>
+        <v>0.672</v>
       </c>
       <c r="I11" t="n">
-        <v>0.1794962859411489</v>
+        <v>0.1499310952849119</v>
       </c>
       <c r="J11" t="n">
-        <v>21.019</v>
+        <v>19.997</v>
       </c>
       <c r="K11" t="n">
-        <v>16.263</v>
+        <v>16.256</v>
       </c>
       <c r="L11" t="n">
-        <v>12.945</v>
+        <v>13.208</v>
       </c>
       <c r="M11" t="n">
-        <v>11.709</v>
+        <v>11.881</v>
       </c>
       <c r="N11" t="n">
-        <v>15.484</v>
+        <v>15.3355</v>
       </c>
       <c r="O11" t="n">
-        <v>4.160937875046922</v>
+        <v>3.607248674544077</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidarctangent_2</t>
+          <t>WLlinear_9</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr">
@@ -1004,47 +1004,47 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>-4.555</v>
+        <v>0.479</v>
       </c>
       <c r="E12" t="n">
-        <v>-1.957</v>
+        <v>0.659</v>
       </c>
       <c r="F12" t="n">
-        <v>-2.049</v>
+        <v>0.756</v>
       </c>
       <c r="G12" t="n">
-        <v>-1.106</v>
+        <v>0.795</v>
       </c>
       <c r="H12" t="n">
-        <v>-2.41675</v>
+        <v>0.67225</v>
       </c>
       <c r="I12" t="n">
-        <v>1.48736778123861</v>
+        <v>0.1409524151383485</v>
       </c>
       <c r="J12" t="n">
-        <v>64.38200000000001</v>
+        <v>19.713</v>
       </c>
       <c r="K12" t="n">
-        <v>48.309</v>
+        <v>16.397</v>
       </c>
       <c r="L12" t="n">
-        <v>46.76</v>
+        <v>13.228</v>
       </c>
       <c r="M12" t="n">
-        <v>38.762</v>
+        <v>12.095</v>
       </c>
       <c r="N12" t="n">
-        <v>49.55325</v>
+        <v>15.35825</v>
       </c>
       <c r="O12" t="n">
-        <v>10.73457508474369</v>
+        <v>3.426835992087551</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidarctangent_3</t>
+          <t>WLpolynomial_10</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr">
@@ -1053,47 +1053,47 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>-0.594</v>
+        <v>0.511</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.627</v>
+        <v>0.597</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.5610000000000001</v>
+        <v>0.679</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.137</v>
+        <v>0.728</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.47975</v>
+        <v>0.62875</v>
       </c>
       <c r="I13" t="n">
-        <v>0.2300831371482925</v>
+        <v>0.09530433708214264</v>
       </c>
       <c r="J13" t="n">
-        <v>34.49</v>
+        <v>19.11</v>
       </c>
       <c r="K13" t="n">
-        <v>35.835</v>
+        <v>17.828</v>
       </c>
       <c r="L13" t="n">
-        <v>33.459</v>
+        <v>15.163</v>
       </c>
       <c r="M13" t="n">
-        <v>28.485</v>
+        <v>13.939</v>
       </c>
       <c r="N13" t="n">
-        <v>33.06725</v>
+        <v>16.51</v>
       </c>
       <c r="O13" t="n">
-        <v>3.205991305353152</v>
+        <v>2.37497887709905</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidarctangent_4</t>
+          <t>WLpolynomial_2</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr">
@@ -1102,47 +1102,47 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>-0.134</v>
+        <v>0.433</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.127</v>
+        <v>0.222</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>0.743</v>
       </c>
       <c r="G14" t="n">
-        <v>0.143</v>
+        <v>0.595</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.02950000000000001</v>
+        <v>0.49825</v>
       </c>
       <c r="I14" t="n">
-        <v>0.1304517790858625</v>
+        <v>0.2234835937304273</v>
       </c>
       <c r="J14" t="n">
-        <v>29.087</v>
+        <v>20.567</v>
       </c>
       <c r="K14" t="n">
-        <v>29.831</v>
+        <v>24.774</v>
       </c>
       <c r="L14" t="n">
-        <v>26.773</v>
+        <v>13.587</v>
       </c>
       <c r="M14" t="n">
-        <v>24.732</v>
+        <v>16.995</v>
       </c>
       <c r="N14" t="n">
-        <v>27.60575</v>
+        <v>18.98075</v>
       </c>
       <c r="O14" t="n">
-        <v>2.316444887465848</v>
+        <v>4.799780437686708</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidarctangent_5</t>
+          <t>WLpolynomial_3</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr">
@@ -1151,47 +1151,47 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.125</v>
+        <v>0.446</v>
       </c>
       <c r="E15" t="n">
-        <v>0.273</v>
+        <v>0.665</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.01</v>
+        <v>0.724</v>
       </c>
       <c r="G15" t="n">
-        <v>0.279</v>
+        <v>0.732</v>
       </c>
       <c r="H15" t="n">
-        <v>0.16675</v>
+        <v>0.64175</v>
       </c>
       <c r="I15" t="n">
-        <v>0.1376865401313191</v>
+        <v>0.1338764978129719</v>
       </c>
       <c r="J15" t="n">
-        <v>25.557</v>
+        <v>20.332</v>
       </c>
       <c r="K15" t="n">
-        <v>23.964</v>
+        <v>16.254</v>
       </c>
       <c r="L15" t="n">
-        <v>26.911</v>
+        <v>14.07</v>
       </c>
       <c r="M15" t="n">
-        <v>22.686</v>
+        <v>13.83</v>
       </c>
       <c r="N15" t="n">
-        <v>24.7795</v>
+        <v>16.1215</v>
       </c>
       <c r="O15" t="n">
-        <v>1.843509424982688</v>
+        <v>3.011394527457337</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidhyperbolictangent_2</t>
+          <t>WLpolynomial_4</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr">
@@ -1200,47 +1200,47 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.251</v>
+        <v>0.4</v>
       </c>
       <c r="E16" t="n">
-        <v>0.433</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="F16" t="n">
-        <v>0.468</v>
+        <v>0.781</v>
       </c>
       <c r="G16" t="n">
-        <v>0.448</v>
+        <v>0.786</v>
       </c>
       <c r="H16" t="n">
-        <v>0.4</v>
+        <v>0.6647500000000001</v>
       </c>
       <c r="I16" t="n">
-        <v>0.1003626756651429</v>
+        <v>0.1817055768727715</v>
       </c>
       <c r="J16" t="n">
-        <v>23.639</v>
+        <v>21.161</v>
       </c>
       <c r="K16" t="n">
-        <v>21.153</v>
+        <v>15.603</v>
       </c>
       <c r="L16" t="n">
-        <v>19.53</v>
+        <v>12.527</v>
       </c>
       <c r="M16" t="n">
-        <v>19.839</v>
+        <v>12.357</v>
       </c>
       <c r="N16" t="n">
-        <v>21.04025</v>
+        <v>15.412</v>
       </c>
       <c r="O16" t="n">
-        <v>1.869943916271287</v>
+        <v>4.112733559730479</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidhyperbolictangent_3</t>
+          <t>WLpolynomial_5</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr">
@@ -1249,47 +1249,47 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.354</v>
+        <v>0.408</v>
       </c>
       <c r="E17" t="n">
-        <v>0.509</v>
+        <v>0.665</v>
       </c>
       <c r="F17" t="n">
-        <v>0.541</v>
+        <v>0.766</v>
       </c>
       <c r="G17" t="n">
-        <v>0.545</v>
+        <v>0.8080000000000001</v>
       </c>
       <c r="H17" t="n">
-        <v>0.48725</v>
+        <v>0.6617500000000001</v>
       </c>
       <c r="I17" t="n">
-        <v>0.09028242723070018</v>
+        <v>0.1794962859411489</v>
       </c>
       <c r="J17" t="n">
-        <v>21.952</v>
+        <v>21.019</v>
       </c>
       <c r="K17" t="n">
-        <v>19.691</v>
+        <v>16.263</v>
       </c>
       <c r="L17" t="n">
-        <v>18.141</v>
+        <v>12.945</v>
       </c>
       <c r="M17" t="n">
-        <v>18.015</v>
+        <v>11.709</v>
       </c>
       <c r="N17" t="n">
-        <v>19.44975</v>
+        <v>15.484</v>
       </c>
       <c r="O17" t="n">
-        <v>1.83401115500061</v>
+        <v>4.160937875046922</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidhyperbolictangent_4</t>
+          <t>WLpolynomial_6</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr">
@@ -1298,47 +1298,47 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.367</v>
+        <v>0.442</v>
       </c>
       <c r="E18" t="n">
-        <v>0.524</v>
+        <v>0.648</v>
       </c>
       <c r="F18" t="n">
-        <v>0.54</v>
+        <v>0.747</v>
       </c>
       <c r="G18" t="n">
-        <v>0.5580000000000001</v>
+        <v>0.797</v>
       </c>
       <c r="H18" t="n">
-        <v>0.49725</v>
+        <v>0.6585000000000001</v>
       </c>
       <c r="I18" t="n">
-        <v>0.087937003966855</v>
+        <v>0.1570530695868969</v>
       </c>
       <c r="J18" t="n">
-        <v>21.725</v>
+        <v>20.411</v>
       </c>
       <c r="K18" t="n">
-        <v>19.38</v>
+        <v>16.666</v>
       </c>
       <c r="L18" t="n">
-        <v>18.162</v>
+        <v>13.457</v>
       </c>
       <c r="M18" t="n">
-        <v>17.752</v>
+        <v>12.032</v>
       </c>
       <c r="N18" t="n">
-        <v>19.25475</v>
+        <v>15.6415</v>
       </c>
       <c r="O18" t="n">
-        <v>1.786074163260493</v>
+        <v>3.723719511456254</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidhyperbolictangent_5</t>
+          <t>WLpolynomial_7</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr">
@@ -1347,47 +1347,47 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.202</v>
+        <v>0.466</v>
       </c>
       <c r="E19" t="n">
-        <v>0.391</v>
+        <v>0.634</v>
       </c>
       <c r="F19" t="n">
-        <v>0.456</v>
+        <v>0.73</v>
       </c>
       <c r="G19" t="n">
-        <v>0.495</v>
+        <v>0.779</v>
       </c>
       <c r="H19" t="n">
-        <v>0.386</v>
+        <v>0.65225</v>
       </c>
       <c r="I19" t="n">
-        <v>0.1299512729192497</v>
+        <v>0.1380009057941287</v>
       </c>
       <c r="J19" t="n">
-        <v>24.4</v>
+        <v>19.963</v>
       </c>
       <c r="K19" t="n">
-        <v>21.925</v>
+        <v>17.008</v>
       </c>
       <c r="L19" t="n">
-        <v>19.754</v>
+        <v>13.909</v>
       </c>
       <c r="M19" t="n">
-        <v>18.979</v>
+        <v>12.556</v>
       </c>
       <c r="N19" t="n">
-        <v>21.2645</v>
+        <v>15.859</v>
       </c>
       <c r="O19" t="n">
-        <v>2.433977608771288</v>
+        <v>3.31035375753106</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidlogistic_2</t>
+          <t>WLpolynomial_8</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr">
@@ -1396,47 +1396,47 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.115</v>
+        <v>0.487</v>
       </c>
       <c r="E20" t="n">
-        <v>0.188</v>
+        <v>0.621</v>
       </c>
       <c r="F20" t="n">
-        <v>0.245</v>
+        <v>0.713</v>
       </c>
       <c r="G20" t="n">
-        <v>0.189</v>
+        <v>0.761</v>
       </c>
       <c r="H20" t="n">
-        <v>0.18425</v>
+        <v>0.6455000000000001</v>
       </c>
       <c r="I20" t="n">
-        <v>0.05330025015576068</v>
+        <v>0.1205805401657608</v>
       </c>
       <c r="J20" t="n">
-        <v>25.702</v>
+        <v>19.569</v>
       </c>
       <c r="K20" t="n">
-        <v>25.325</v>
+        <v>17.298</v>
       </c>
       <c r="L20" t="n">
-        <v>23.269</v>
+        <v>14.341</v>
       </c>
       <c r="M20" t="n">
-        <v>24.049</v>
+        <v>13.055</v>
       </c>
       <c r="N20" t="n">
-        <v>24.58625</v>
+        <v>16.06575</v>
       </c>
       <c r="O20" t="n">
-        <v>1.127598443595947</v>
+        <v>2.934313022952164</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidlogistic_3</t>
+          <t>WLpolynomial_9</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr">
@@ -1445,47 +1445,47 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.207</v>
+        <v>0.501</v>
       </c>
       <c r="E21" t="n">
-        <v>0.295</v>
+        <v>0.609</v>
       </c>
       <c r="F21" t="n">
-        <v>0.363</v>
+        <v>0.696</v>
       </c>
       <c r="G21" t="n">
-        <v>0.313</v>
+        <v>0.744</v>
       </c>
       <c r="H21" t="n">
-        <v>0.2945</v>
+        <v>0.6375</v>
       </c>
       <c r="I21" t="n">
-        <v>0.06504101270224298</v>
+        <v>0.1067848303833461</v>
       </c>
       <c r="J21" t="n">
-        <v>24.326</v>
+        <v>19.296</v>
       </c>
       <c r="K21" t="n">
-        <v>23.585</v>
+        <v>17.562</v>
       </c>
       <c r="L21" t="n">
-        <v>21.378</v>
+        <v>14.758</v>
       </c>
       <c r="M21" t="n">
-        <v>22.133</v>
+        <v>13.512</v>
       </c>
       <c r="N21" t="n">
-        <v>22.8555</v>
+        <v>16.282</v>
       </c>
       <c r="O21" t="n">
-        <v>1.341585256329243</v>
+        <v>2.627931505956729</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidlogistic_4</t>
+          <t>WLrbf_10</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr">
@@ -1494,47 +1494,47 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.242</v>
+        <v>-0.012</v>
       </c>
       <c r="E22" t="n">
-        <v>0.342</v>
+        <v>0.01</v>
       </c>
       <c r="F22" t="n">
-        <v>0.397</v>
+        <v>0.01</v>
       </c>
       <c r="G22" t="n">
-        <v>0.358</v>
+        <v>-0.01</v>
       </c>
       <c r="H22" t="n">
-        <v>0.33475</v>
+        <v>-0.0005</v>
       </c>
       <c r="I22" t="n">
-        <v>0.06600694407913964</v>
+        <v>0.01215181742237212</v>
       </c>
       <c r="J22" t="n">
-        <v>23.782</v>
+        <v>27.484</v>
       </c>
       <c r="K22" t="n">
-        <v>22.789</v>
+        <v>27.957</v>
       </c>
       <c r="L22" t="n">
-        <v>20.789</v>
+        <v>26.649</v>
       </c>
       <c r="M22" t="n">
-        <v>21.394</v>
+        <v>26.849</v>
       </c>
       <c r="N22" t="n">
-        <v>22.1885</v>
+        <v>27.23475</v>
       </c>
       <c r="O22" t="n">
-        <v>1.352734637687673</v>
+        <v>0.598797893004532</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidlogistic_5</t>
+          <t>WLrbf_2</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr">
@@ -1543,47 +1543,831 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.271</v>
+        <v>0.162</v>
       </c>
       <c r="E23" t="n">
-        <v>0.365</v>
+        <v>0.137</v>
       </c>
       <c r="F23" t="n">
-        <v>0.422</v>
+        <v>0.146</v>
       </c>
       <c r="G23" t="n">
-        <v>0.382</v>
+        <v>0.104</v>
       </c>
       <c r="H23" t="n">
-        <v>0.36</v>
+        <v>0.13725</v>
       </c>
       <c r="I23" t="n">
-        <v>0.06396353127629315</v>
+        <v>0.02445914961727002</v>
       </c>
       <c r="J23" t="n">
-        <v>23.326</v>
+        <v>25.004</v>
       </c>
       <c r="K23" t="n">
-        <v>22.386</v>
+        <v>26.102</v>
       </c>
       <c r="L23" t="n">
-        <v>20.355</v>
+        <v>24.744</v>
       </c>
       <c r="M23" t="n">
-        <v>20.996</v>
+        <v>25.278</v>
       </c>
       <c r="N23" t="n">
-        <v>21.76575</v>
+        <v>25.282</v>
       </c>
       <c r="O23" t="n">
-        <v>1.341866951924321</v>
+        <v>0.5885417005899696</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n"/>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>WLrbf_3</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-0.026</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-0.056</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.106</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.064</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.1322724461102916</v>
+      </c>
+      <c r="J24" t="n">
+        <v>23.935</v>
+      </c>
+      <c r="K24" t="n">
+        <v>28.454</v>
+      </c>
+      <c r="L24" t="n">
+        <v>27.515</v>
+      </c>
+      <c r="M24" t="n">
+        <v>25.252</v>
+      </c>
+      <c r="N24" t="n">
+        <v>26.289</v>
+      </c>
+      <c r="O24" t="n">
+        <v>2.066154721537895</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n"/>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>WLrbf_4</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.189</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.147</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.186</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.13325</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.08371529131526689</v>
+      </c>
+      <c r="J25" t="n">
+        <v>24.595</v>
+      </c>
+      <c r="K25" t="n">
+        <v>25.945</v>
+      </c>
+      <c r="L25" t="n">
+        <v>26.634</v>
+      </c>
+      <c r="M25" t="n">
+        <v>24.098</v>
+      </c>
+      <c r="N25" t="n">
+        <v>25.318</v>
+      </c>
+      <c r="O25" t="n">
+        <v>1.174182552530342</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n"/>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>WLrbf_5</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.157</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.163</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.15525</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.009810708435174299</v>
+      </c>
+      <c r="J26" t="n">
+        <v>25.32</v>
+      </c>
+      <c r="K26" t="n">
+        <v>25.75</v>
+      </c>
+      <c r="L26" t="n">
+        <v>24.589</v>
+      </c>
+      <c r="M26" t="n">
+        <v>24.436</v>
+      </c>
+      <c r="N26" t="n">
+        <v>25.02375</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0.619047857600687</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n"/>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>WLrbf_6</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.132</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.094</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.104</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.03080043289739069</v>
+      </c>
+      <c r="J27" t="n">
+        <v>26.412</v>
+      </c>
+      <c r="K27" t="n">
+        <v>26.288</v>
+      </c>
+      <c r="L27" t="n">
+        <v>24.956</v>
+      </c>
+      <c r="M27" t="n">
+        <v>25.42</v>
+      </c>
+      <c r="N27" t="n">
+        <v>25.769</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0.6989468267805972</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n"/>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>WLrbf_7</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.083</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.08400000000000001</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.05875</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.02995969514753669</v>
+      </c>
+      <c r="J28" t="n">
+        <v>27.002</v>
+      </c>
+      <c r="K28" t="n">
+        <v>26.906</v>
+      </c>
+      <c r="L28" t="n">
+        <v>25.625</v>
+      </c>
+      <c r="M28" t="n">
+        <v>26.102</v>
+      </c>
+      <c r="N28" t="n">
+        <v>26.40875</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0.660192585538492</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n"/>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>WLrbf_8</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.02825</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.02309942279221135</v>
+      </c>
+      <c r="J29" t="n">
+        <v>27.261</v>
+      </c>
+      <c r="K29" t="n">
+        <v>27.407</v>
+      </c>
+      <c r="L29" t="n">
+        <v>26.134</v>
+      </c>
+      <c r="M29" t="n">
+        <v>26.536</v>
+      </c>
+      <c r="N29" t="n">
+        <v>26.8345</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0.6026223250649332</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n"/>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>WLrbf_9</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>-0.005</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="G30" t="n">
+        <v>-0.006</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.01675310916417208</v>
+      </c>
+      <c r="J30" t="n">
+        <v>27.382</v>
+      </c>
+      <c r="K30" t="n">
+        <v>27.75</v>
+      </c>
+      <c r="L30" t="n">
+        <v>26.467</v>
+      </c>
+      <c r="M30" t="n">
+        <v>26.783</v>
+      </c>
+      <c r="N30" t="n">
+        <v>27.0955</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0.5782505224093336</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n"/>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_10</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.473</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.648</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.749</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.6082500000000001</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.11794172289737</v>
+      </c>
+      <c r="J31" t="n">
+        <v>19.828</v>
+      </c>
+      <c r="K31" t="n">
+        <v>18.572</v>
+      </c>
+      <c r="L31" t="n">
+        <v>15.888</v>
+      </c>
+      <c r="M31" t="n">
+        <v>13.375</v>
+      </c>
+      <c r="N31" t="n">
+        <v>16.91575</v>
+      </c>
+      <c r="O31" t="n">
+        <v>2.876197996777458</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n"/>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_2</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.251</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.433</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.468</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.448</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.1003626756651429</v>
+      </c>
+      <c r="J32" t="n">
+        <v>23.639</v>
+      </c>
+      <c r="K32" t="n">
+        <v>21.153</v>
+      </c>
+      <c r="L32" t="n">
+        <v>19.53</v>
+      </c>
+      <c r="M32" t="n">
+        <v>19.839</v>
+      </c>
+      <c r="N32" t="n">
+        <v>21.04025</v>
+      </c>
+      <c r="O32" t="n">
+        <v>1.869943916271287</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n"/>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_3</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.354</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.509</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.541</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.545</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.48725</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.09028242723070018</v>
+      </c>
+      <c r="J33" t="n">
+        <v>21.952</v>
+      </c>
+      <c r="K33" t="n">
+        <v>19.691</v>
+      </c>
+      <c r="L33" t="n">
+        <v>18.141</v>
+      </c>
+      <c r="M33" t="n">
+        <v>18.015</v>
+      </c>
+      <c r="N33" t="n">
+        <v>19.44975</v>
+      </c>
+      <c r="O33" t="n">
+        <v>1.83401115500061</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n"/>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_4</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.367</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.5580000000000001</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.49725</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.087937003966855</v>
+      </c>
+      <c r="J34" t="n">
+        <v>21.725</v>
+      </c>
+      <c r="K34" t="n">
+        <v>19.38</v>
+      </c>
+      <c r="L34" t="n">
+        <v>18.162</v>
+      </c>
+      <c r="M34" t="n">
+        <v>17.752</v>
+      </c>
+      <c r="N34" t="n">
+        <v>19.25475</v>
+      </c>
+      <c r="O34" t="n">
+        <v>1.786074163260493</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n"/>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_5</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.202</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.391</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.456</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.495</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.386</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.1299512729192497</v>
+      </c>
+      <c r="J35" t="n">
+        <v>24.4</v>
+      </c>
+      <c r="K35" t="n">
+        <v>21.925</v>
+      </c>
+      <c r="L35" t="n">
+        <v>19.754</v>
+      </c>
+      <c r="M35" t="n">
+        <v>18.979</v>
+      </c>
+      <c r="N35" t="n">
+        <v>21.2645</v>
+      </c>
+      <c r="O35" t="n">
+        <v>2.433977608771288</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n"/>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_6</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.409</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.677</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.712</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.5902499999999999</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.1365561545055123</v>
+      </c>
+      <c r="J36" t="n">
+        <v>21.006</v>
+      </c>
+      <c r="K36" t="n">
+        <v>18.581</v>
+      </c>
+      <c r="L36" t="n">
+        <v>15.212</v>
+      </c>
+      <c r="M36" t="n">
+        <v>14.325</v>
+      </c>
+      <c r="N36" t="n">
+        <v>17.281</v>
+      </c>
+      <c r="O36" t="n">
+        <v>3.086763245429318</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n"/>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_7</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.607</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.695</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.613</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.1312732519086301</v>
+      </c>
+      <c r="J37" t="n">
+        <v>20.625</v>
+      </c>
+      <c r="K37" t="n">
+        <v>17.616</v>
+      </c>
+      <c r="L37" t="n">
+        <v>14.796</v>
+      </c>
+      <c r="M37" t="n">
+        <v>14.138</v>
+      </c>
+      <c r="N37" t="n">
+        <v>16.79375</v>
+      </c>
+      <c r="O37" t="n">
+        <v>2.966399880326319</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n"/>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_8</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.444</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.612</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.694</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.61875</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.1258765930054777</v>
+      </c>
+      <c r="J38" t="n">
+        <v>20.372</v>
+      </c>
+      <c r="K38" t="n">
+        <v>17.49</v>
+      </c>
+      <c r="L38" t="n">
+        <v>14.808</v>
+      </c>
+      <c r="M38" t="n">
+        <v>13.995</v>
+      </c>
+      <c r="N38" t="n">
+        <v>16.66625</v>
+      </c>
+      <c r="O38" t="n">
+        <v>2.886740765985058</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n"/>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_9</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.142</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-0.333</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-0.449</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.722</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.02049999999999999</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.532996873036481</v>
+      </c>
+      <c r="J39" t="n">
+        <v>25.296</v>
+      </c>
+      <c r="K39" t="n">
+        <v>32.441</v>
+      </c>
+      <c r="L39" t="n">
+        <v>32.229</v>
+      </c>
+      <c r="M39" t="n">
+        <v>14.083</v>
+      </c>
+      <c r="N39" t="n">
+        <v>26.01225</v>
+      </c>
+      <c r="O39" t="n">
+        <v>8.617749643420066</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="J1:O1"/>
-    <mergeCell ref="A4:A23"/>
+    <mergeCell ref="A4:A39"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -1595,7 +2379,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1710,7 +2494,7 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>WLlinear_2</t>
+          <t>WLlinear_10</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
@@ -1719,41 +2503,41 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.62</v>
+        <v>0.486</v>
       </c>
       <c r="E4" t="n">
-        <v>0.439</v>
+        <v>0.574</v>
       </c>
       <c r="F4" t="n">
-        <v>0.348</v>
+        <v>0.522</v>
       </c>
       <c r="G4" t="n">
-        <v>0.469</v>
+        <v>0.5273333333333333</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1384593803250614</v>
+        <v>0.04424176006143214</v>
       </c>
       <c r="I4" t="n">
-        <v>15.349</v>
+        <v>17.858</v>
       </c>
       <c r="J4" t="n">
-        <v>19.955</v>
+        <v>17.381</v>
       </c>
       <c r="K4" t="n">
-        <v>21.389</v>
+        <v>18.319</v>
       </c>
       <c r="L4" t="n">
-        <v>18.89766666666667</v>
+        <v>17.85266666666667</v>
       </c>
       <c r="M4" t="n">
-        <v>3.155766996046021</v>
+        <v>0.4690227428743011</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>WLlinear_3</t>
+          <t>WLlinear_2</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
@@ -1762,41 +2546,41 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.652</v>
+        <v>0.62</v>
       </c>
       <c r="E5" t="n">
-        <v>0.652</v>
+        <v>0.439</v>
       </c>
       <c r="F5" t="n">
-        <v>0.673</v>
+        <v>0.348</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6590000000000001</v>
+        <v>0.469</v>
       </c>
       <c r="H5" t="n">
-        <v>0.01212435565298215</v>
+        <v>0.1384593803250614</v>
       </c>
       <c r="I5" t="n">
-        <v>14.693</v>
+        <v>15.349</v>
       </c>
       <c r="J5" t="n">
-        <v>15.707</v>
+        <v>19.955</v>
       </c>
       <c r="K5" t="n">
-        <v>15.16</v>
+        <v>21.389</v>
       </c>
       <c r="L5" t="n">
-        <v>15.18666666666667</v>
+        <v>18.89766666666667</v>
       </c>
       <c r="M5" t="n">
-        <v>0.5075256972147656</v>
+        <v>3.155766996046021</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>WLlinear_4</t>
+          <t>WLlinear_3</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
@@ -1805,41 +2589,41 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.654</v>
+        <v>0.652</v>
       </c>
       <c r="E6" t="n">
-        <v>0.661</v>
+        <v>0.652</v>
       </c>
       <c r="F6" t="n">
-        <v>0.658</v>
+        <v>0.673</v>
       </c>
       <c r="G6" t="n">
-        <v>0.6576666666666666</v>
+        <v>0.6590000000000001</v>
       </c>
       <c r="H6" t="n">
-        <v>0.00351188458428425</v>
+        <v>0.01212435565298215</v>
       </c>
       <c r="I6" t="n">
-        <v>14.646</v>
+        <v>14.693</v>
       </c>
       <c r="J6" t="n">
-        <v>15.516</v>
+        <v>15.707</v>
       </c>
       <c r="K6" t="n">
-        <v>15.488</v>
+        <v>15.16</v>
       </c>
       <c r="L6" t="n">
-        <v>15.21666666666667</v>
+        <v>15.18666666666667</v>
       </c>
       <c r="M6" t="n">
-        <v>0.4944100861970079</v>
+        <v>0.5075256972147656</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>WLlinear_5</t>
+          <t>WLlinear_4</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
@@ -1848,41 +2632,41 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.63</v>
+        <v>0.654</v>
       </c>
       <c r="E7" t="n">
-        <v>0.707</v>
+        <v>0.661</v>
       </c>
       <c r="F7" t="n">
-        <v>0.614</v>
+        <v>0.658</v>
       </c>
       <c r="G7" t="n">
-        <v>0.6503333333333333</v>
+        <v>0.6576666666666666</v>
       </c>
       <c r="H7" t="n">
-        <v>0.04972256362390551</v>
+        <v>0.00351188458428425</v>
       </c>
       <c r="I7" t="n">
-        <v>15.162</v>
+        <v>14.646</v>
       </c>
       <c r="J7" t="n">
-        <v>14.427</v>
+        <v>15.516</v>
       </c>
       <c r="K7" t="n">
-        <v>16.453</v>
+        <v>15.488</v>
       </c>
       <c r="L7" t="n">
-        <v>15.34733333333333</v>
+        <v>15.21666666666667</v>
       </c>
       <c r="M7" t="n">
-        <v>1.025636550310749</v>
+        <v>0.4944100861970079</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>WLpolynomial_2</t>
+          <t>WLlinear_5</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
@@ -1891,41 +2675,41 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.656</v>
+        <v>0.63</v>
       </c>
       <c r="E8" t="n">
-        <v>0.434</v>
+        <v>0.707</v>
       </c>
       <c r="F8" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.614</v>
       </c>
       <c r="G8" t="n">
-        <v>0.3923333333333334</v>
+        <v>0.6503333333333333</v>
       </c>
       <c r="H8" t="n">
-        <v>0.2867792414616744</v>
+        <v>0.04972256362390551</v>
       </c>
       <c r="I8" t="n">
-        <v>14.605</v>
+        <v>15.162</v>
       </c>
       <c r="J8" t="n">
-        <v>20.039</v>
+        <v>14.427</v>
       </c>
       <c r="K8" t="n">
-        <v>25.317</v>
+        <v>16.453</v>
       </c>
       <c r="L8" t="n">
-        <v>19.987</v>
+        <v>15.34733333333333</v>
       </c>
       <c r="M8" t="n">
-        <v>5.356189317042481</v>
+        <v>1.025636550310749</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>WLpolynomial_3</t>
+          <t>WLlinear_6</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr">
@@ -1934,41 +2718,41 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.652</v>
+        <v>0.591</v>
       </c>
       <c r="E9" t="n">
-        <v>0.6840000000000001</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="F9" t="n">
-        <v>0.655</v>
+        <v>0.588</v>
       </c>
       <c r="G9" t="n">
-        <v>0.6636666666666667</v>
+        <v>0.6236666666666666</v>
       </c>
       <c r="H9" t="n">
-        <v>0.01767295485574876</v>
+        <v>0.05919740985324723</v>
       </c>
       <c r="I9" t="n">
-        <v>14.708</v>
+        <v>15.935</v>
       </c>
       <c r="J9" t="n">
-        <v>14.98</v>
+        <v>14.787</v>
       </c>
       <c r="K9" t="n">
-        <v>15.554</v>
+        <v>17.002</v>
       </c>
       <c r="L9" t="n">
-        <v>15.08066666666667</v>
+        <v>15.908</v>
       </c>
       <c r="M9" t="n">
-        <v>0.4318904182004196</v>
+        <v>1.107746812227414</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>WLpolynomial_4</t>
+          <t>WLlinear_7</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr">
@@ -1977,41 +2761,41 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.653</v>
+        <v>0.555</v>
       </c>
       <c r="E10" t="n">
         <v>0.667</v>
       </c>
       <c r="F10" t="n">
-        <v>0.638</v>
+        <v>0.572</v>
       </c>
       <c r="G10" t="n">
-        <v>0.6526666666666667</v>
+        <v>0.598</v>
       </c>
       <c r="H10" t="n">
-        <v>0.01450287327853807</v>
+        <v>0.06035726965329033</v>
       </c>
       <c r="I10" t="n">
-        <v>14.684</v>
+        <v>16.621</v>
       </c>
       <c r="J10" t="n">
-        <v>15.373</v>
+        <v>15.382</v>
       </c>
       <c r="K10" t="n">
-        <v>15.932</v>
+        <v>17.339</v>
       </c>
       <c r="L10" t="n">
-        <v>15.32966666666667</v>
+        <v>16.44733333333333</v>
       </c>
       <c r="M10" t="n">
-        <v>0.6251274536711166</v>
+        <v>0.9899910774008684</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>WLpolynomial_5</t>
+          <t>WLlinear_8</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr">
@@ -2020,41 +2804,41 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.59</v>
+        <v>0.527</v>
       </c>
       <c r="E11" t="n">
-        <v>0.656</v>
+        <v>0.631</v>
       </c>
       <c r="F11" t="n">
-        <v>0.579</v>
+        <v>0.552</v>
       </c>
       <c r="G11" t="n">
-        <v>0.6083333333333333</v>
+        <v>0.57</v>
       </c>
       <c r="H11" t="n">
-        <v>0.04164532786920205</v>
+        <v>0.05428627819255984</v>
       </c>
       <c r="I11" t="n">
-        <v>15.945</v>
+        <v>17.136</v>
       </c>
       <c r="J11" t="n">
-        <v>15.623</v>
+        <v>16.173</v>
       </c>
       <c r="K11" t="n">
-        <v>17.187</v>
+        <v>17.734</v>
       </c>
       <c r="L11" t="n">
-        <v>16.25166666666667</v>
+        <v>17.01433333333333</v>
       </c>
       <c r="M11" t="n">
-        <v>0.8258676245823751</v>
+        <v>0.7875800488415994</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidarctangent_2</t>
+          <t>WLlinear_9</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr">
@@ -2063,41 +2847,41 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>-2.025</v>
+        <v>0.505</v>
       </c>
       <c r="E12" t="n">
-        <v>-2.106</v>
+        <v>0.6</v>
       </c>
       <c r="F12" t="n">
-        <v>-2.23</v>
+        <v>0.536</v>
       </c>
       <c r="G12" t="n">
-        <v>-2.120333333333333</v>
+        <v>0.547</v>
       </c>
       <c r="H12" t="n">
-        <v>0.1032488902280956</v>
+        <v>0.04844584605515728</v>
       </c>
       <c r="I12" t="n">
-        <v>43.335</v>
+        <v>17.535</v>
       </c>
       <c r="J12" t="n">
-        <v>46.953</v>
+        <v>16.839</v>
       </c>
       <c r="K12" t="n">
-        <v>47.615</v>
+        <v>18.055</v>
       </c>
       <c r="L12" t="n">
-        <v>45.96766666666667</v>
+        <v>17.47633333333333</v>
       </c>
       <c r="M12" t="n">
-        <v>2.30385792386018</v>
+        <v>0.6101191140534232</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidarctangent_3</t>
+          <t>WLpolynomial_10</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr">
@@ -2106,41 +2890,41 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>-0.14</v>
+        <v>0.411</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.347</v>
+        <v>0.424</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.291</v>
+        <v>0.419</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.2593333333333333</v>
+        <v>0.418</v>
       </c>
       <c r="H13" t="n">
-        <v>0.1070716271163063</v>
+        <v>0.006557438524302007</v>
       </c>
       <c r="I13" t="n">
-        <v>26.6</v>
+        <v>19.122</v>
       </c>
       <c r="J13" t="n">
-        <v>30.916</v>
+        <v>20.222</v>
       </c>
       <c r="K13" t="n">
-        <v>30.109</v>
+        <v>20.187</v>
       </c>
       <c r="L13" t="n">
-        <v>29.20833333333333</v>
+        <v>19.84366666666667</v>
       </c>
       <c r="M13" t="n">
-        <v>2.294638170460287</v>
+        <v>0.6252266255793448</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidarctangent_4</t>
+          <t>WLpolynomial_2</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr">
@@ -2149,41 +2933,41 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>-0.099</v>
+        <v>0.656</v>
       </c>
       <c r="E14" t="n">
-        <v>0.25</v>
+        <v>0.434</v>
       </c>
       <c r="F14" t="n">
-        <v>0.176</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="G14" t="n">
-        <v>0.109</v>
+        <v>0.3923333333333334</v>
       </c>
       <c r="H14" t="n">
-        <v>0.1838939912014528</v>
+        <v>0.2867792414616744</v>
       </c>
       <c r="I14" t="n">
-        <v>26.125</v>
+        <v>14.605</v>
       </c>
       <c r="J14" t="n">
-        <v>23.071</v>
+        <v>20.039</v>
       </c>
       <c r="K14" t="n">
-        <v>24.053</v>
+        <v>25.317</v>
       </c>
       <c r="L14" t="n">
-        <v>24.41633333333333</v>
+        <v>19.987</v>
       </c>
       <c r="M14" t="n">
-        <v>1.559082208651401</v>
+        <v>5.356189317042481</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidarctangent_5</t>
+          <t>WLpolynomial_3</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr">
@@ -2192,41 +2976,41 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.164</v>
+        <v>0.652</v>
       </c>
       <c r="E15" t="n">
-        <v>0.142</v>
+        <v>0.6840000000000001</v>
       </c>
       <c r="F15" t="n">
-        <v>0.031</v>
+        <v>0.655</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1123333333333333</v>
+        <v>0.6636666666666667</v>
       </c>
       <c r="H15" t="n">
-        <v>0.07129048557369583</v>
+        <v>0.01767295485574876</v>
       </c>
       <c r="I15" t="n">
-        <v>22.778</v>
+        <v>14.708</v>
       </c>
       <c r="J15" t="n">
-        <v>24.679</v>
+        <v>14.98</v>
       </c>
       <c r="K15" t="n">
-        <v>26.076</v>
+        <v>15.554</v>
       </c>
       <c r="L15" t="n">
-        <v>24.511</v>
+        <v>15.08066666666667</v>
       </c>
       <c r="M15" t="n">
-        <v>1.655405992498518</v>
+        <v>0.4318904182004196</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidhyperbolictangent_2</t>
+          <t>WLpolynomial_4</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr">
@@ -2235,41 +3019,41 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.334</v>
+        <v>0.653</v>
       </c>
       <c r="E16" t="n">
-        <v>0.468</v>
+        <v>0.667</v>
       </c>
       <c r="F16" t="n">
-        <v>0.249</v>
+        <v>0.638</v>
       </c>
       <c r="G16" t="n">
-        <v>0.3503333333333334</v>
+        <v>0.6526666666666667</v>
       </c>
       <c r="H16" t="n">
-        <v>0.1104098425564195</v>
+        <v>0.01450287327853807</v>
       </c>
       <c r="I16" t="n">
-        <v>20.325</v>
+        <v>14.684</v>
       </c>
       <c r="J16" t="n">
-        <v>19.435</v>
+        <v>15.373</v>
       </c>
       <c r="K16" t="n">
-        <v>22.962</v>
+        <v>15.932</v>
       </c>
       <c r="L16" t="n">
-        <v>20.90733333333333</v>
+        <v>15.32966666666667</v>
       </c>
       <c r="M16" t="n">
-        <v>1.834193646628767</v>
+        <v>0.6251274536711166</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidhyperbolictangent_3</t>
+          <t>WLpolynomial_5</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr">
@@ -2278,41 +3062,41 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.44</v>
+        <v>0.59</v>
       </c>
       <c r="E17" t="n">
-        <v>0.522</v>
+        <v>0.656</v>
       </c>
       <c r="F17" t="n">
-        <v>0.381</v>
+        <v>0.579</v>
       </c>
       <c r="G17" t="n">
-        <v>0.4476666666666667</v>
+        <v>0.6083333333333333</v>
       </c>
       <c r="H17" t="n">
-        <v>0.07081195755896977</v>
+        <v>0.04164532786920205</v>
       </c>
       <c r="I17" t="n">
-        <v>18.643</v>
+        <v>15.945</v>
       </c>
       <c r="J17" t="n">
-        <v>18.428</v>
+        <v>15.623</v>
       </c>
       <c r="K17" t="n">
-        <v>20.841</v>
+        <v>17.187</v>
       </c>
       <c r="L17" t="n">
-        <v>19.304</v>
+        <v>16.25166666666667</v>
       </c>
       <c r="M17" t="n">
-        <v>1.335414916795526</v>
+        <v>0.8258676245823751</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidhyperbolictangent_4</t>
+          <t>WLpolynomial_6</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr">
@@ -2321,41 +3105,41 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.421</v>
+        <v>0.534</v>
       </c>
       <c r="E18" t="n">
-        <v>0.486</v>
+        <v>0.609</v>
       </c>
       <c r="F18" t="n">
-        <v>0.357</v>
+        <v>0.538</v>
       </c>
       <c r="G18" t="n">
-        <v>0.4213333333333333</v>
+        <v>0.5603333333333333</v>
       </c>
       <c r="H18" t="n">
-        <v>0.06450064599159712</v>
+        <v>0.04219399641339193</v>
       </c>
       <c r="I18" t="n">
-        <v>18.955</v>
+        <v>17.011</v>
       </c>
       <c r="J18" t="n">
-        <v>19.091</v>
+        <v>16.663</v>
       </c>
       <c r="K18" t="n">
-        <v>21.254</v>
+        <v>18.015</v>
       </c>
       <c r="L18" t="n">
-        <v>19.76666666666667</v>
+        <v>17.22966666666666</v>
       </c>
       <c r="M18" t="n">
-        <v>1.289862137336133</v>
+        <v>0.7020237412889494</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidhyperbolictangent_5</t>
+          <t>WLpolynomial_7</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr">
@@ -2364,41 +3148,41 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.509</v>
+        <v>0.499</v>
       </c>
       <c r="E19" t="n">
-        <v>0.416</v>
+        <v>0.548</v>
       </c>
       <c r="F19" t="n">
-        <v>0.304</v>
+        <v>0.503</v>
       </c>
       <c r="G19" t="n">
-        <v>0.4096666666666667</v>
+        <v>0.5166666666666667</v>
       </c>
       <c r="H19" t="n">
-        <v>0.1026466430689934</v>
+        <v>0.02720906711619005</v>
       </c>
       <c r="I19" t="n">
-        <v>17.461</v>
+        <v>17.64</v>
       </c>
       <c r="J19" t="n">
-        <v>20.361</v>
+        <v>17.903</v>
       </c>
       <c r="K19" t="n">
-        <v>22.098</v>
+        <v>18.682</v>
       </c>
       <c r="L19" t="n">
-        <v>19.97333333333333</v>
+        <v>18.075</v>
       </c>
       <c r="M19" t="n">
-        <v>2.342681440856468</v>
+        <v>0.5418754469432981</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidlogistic_2</t>
+          <t>WLpolynomial_8</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr">
@@ -2407,41 +3191,41 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.097</v>
+        <v>0.464</v>
       </c>
       <c r="E20" t="n">
-        <v>0.227</v>
+        <v>0.499</v>
       </c>
       <c r="F20" t="n">
-        <v>0.06900000000000001</v>
+        <v>0.473</v>
       </c>
       <c r="G20" t="n">
-        <v>0.131</v>
+        <v>0.4786666666666666</v>
       </c>
       <c r="H20" t="n">
-        <v>0.08430895563343198</v>
+        <v>0.01817507450695411</v>
       </c>
       <c r="I20" t="n">
-        <v>23.681</v>
+        <v>18.235</v>
       </c>
       <c r="J20" t="n">
-        <v>23.429</v>
+        <v>18.86</v>
       </c>
       <c r="K20" t="n">
-        <v>25.572</v>
+        <v>19.243</v>
       </c>
       <c r="L20" t="n">
-        <v>24.22733333333333</v>
+        <v>18.77933333333333</v>
       </c>
       <c r="M20" t="n">
-        <v>1.171312227091194</v>
+        <v>0.5088185662231017</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidlogistic_3</t>
+          <t>WLpolynomial_9</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr">
@@ -2450,41 +3234,41 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.213</v>
+        <v>0.436</v>
       </c>
       <c r="E21" t="n">
-        <v>0.299</v>
+        <v>0.458</v>
       </c>
       <c r="F21" t="n">
-        <v>0.158</v>
+        <v>0.445</v>
       </c>
       <c r="G21" t="n">
-        <v>0.2233333333333333</v>
+        <v>0.4463333333333333</v>
       </c>
       <c r="H21" t="n">
-        <v>0.07106569730420811</v>
+        <v>0.01106044001535805</v>
       </c>
       <c r="I21" t="n">
-        <v>22.102</v>
+        <v>18.715</v>
       </c>
       <c r="J21" t="n">
-        <v>22.312</v>
+        <v>19.609</v>
       </c>
       <c r="K21" t="n">
-        <v>24.309</v>
+        <v>19.736</v>
       </c>
       <c r="L21" t="n">
-        <v>22.90766666666667</v>
+        <v>19.35333333333334</v>
       </c>
       <c r="M21" t="n">
-        <v>1.218124104241162</v>
+        <v>0.5564479610290024</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidlogistic_4</t>
+          <t>WLrbf_10</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr">
@@ -2493,41 +3277,41 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.245</v>
+        <v>-0.004</v>
       </c>
       <c r="E22" t="n">
-        <v>0.303</v>
+        <v>0.004</v>
       </c>
       <c r="F22" t="n">
-        <v>0.168</v>
+        <v>-0.005</v>
       </c>
       <c r="G22" t="n">
-        <v>0.2386666666666667</v>
+        <v>-0.001666666666666667</v>
       </c>
       <c r="H22" t="n">
-        <v>0.06772247288259144</v>
+        <v>0.004932882862316247</v>
       </c>
       <c r="I22" t="n">
-        <v>21.654</v>
+        <v>24.963</v>
       </c>
       <c r="J22" t="n">
-        <v>22.235</v>
+        <v>26.586</v>
       </c>
       <c r="K22" t="n">
-        <v>24.172</v>
+        <v>26.563</v>
       </c>
       <c r="L22" t="n">
-        <v>22.687</v>
+        <v>26.03733333333333</v>
       </c>
       <c r="M22" t="n">
-        <v>1.318449468125344</v>
+        <v>0.9304710276700349</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>WLsigmoidlogistic_5</t>
+          <t>WLrbf_2</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr">
@@ -2536,41 +3320,729 @@
         </is>
       </c>
       <c r="D23" t="n">
+        <v>0.154</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.198</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.04303486958270002</v>
+      </c>
+      <c r="I23" t="n">
+        <v>22.922</v>
+      </c>
+      <c r="J23" t="n">
+        <v>23.223</v>
+      </c>
+      <c r="K23" t="n">
+        <v>23.699</v>
+      </c>
+      <c r="L23" t="n">
+        <v>23.28133333333333</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.3917707663077145</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n"/>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>WLrbf_3</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.149</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.1996666666666667</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.04416257842714048</v>
+      </c>
+      <c r="I24" t="n">
+        <v>22.004</v>
+      </c>
+      <c r="J24" t="n">
+        <v>23.383</v>
+      </c>
+      <c r="K24" t="n">
+        <v>24.444</v>
+      </c>
+      <c r="L24" t="n">
+        <v>23.277</v>
+      </c>
+      <c r="M24" t="n">
+        <v>1.223448813804647</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n"/>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>WLrbf_4</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.117</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.225</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.184</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.1753333333333333</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.05451910979953115</v>
+      </c>
+      <c r="I25" t="n">
+        <v>23.407</v>
+      </c>
+      <c r="J25" t="n">
+        <v>23.456</v>
+      </c>
+      <c r="K25" t="n">
+        <v>23.939</v>
+      </c>
+      <c r="L25" t="n">
+        <v>23.60066666666667</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.2940277764656486</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n"/>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>WLrbf_5</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.182</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.189</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.139</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.08061637550770935</v>
+      </c>
+      <c r="I26" t="n">
+        <v>24.329</v>
+      </c>
+      <c r="J26" t="n">
+        <v>24.095</v>
+      </c>
+      <c r="K26" t="n">
+        <v>23.86</v>
+      </c>
+      <c r="L26" t="n">
+        <v>24.09466666666667</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.2345001776829468</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n"/>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>WLrbf_6</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.145</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.165</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.1036666666666667</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.08947252837230729</v>
+      </c>
+      <c r="I27" t="n">
+        <v>24.904</v>
+      </c>
+      <c r="J27" t="n">
+        <v>24.633</v>
+      </c>
+      <c r="K27" t="n">
+        <v>24.207</v>
+      </c>
+      <c r="L27" t="n">
+        <v>24.58133333333333</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.3513606883721242</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n"/>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>WLrbf_7</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.091</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.105</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.05758472019555187</v>
+      </c>
+      <c r="I28" t="n">
+        <v>24.93</v>
+      </c>
+      <c r="J28" t="n">
+        <v>25.405</v>
+      </c>
+      <c r="K28" t="n">
+        <v>25.064</v>
+      </c>
+      <c r="L28" t="n">
+        <v>25.133</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.2449020212248163</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n"/>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>WLrbf_8</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="I29" t="n">
+        <v>24.911</v>
+      </c>
+      <c r="J29" t="n">
+        <v>26.048</v>
+      </c>
+      <c r="K29" t="n">
+        <v>25.882</v>
+      </c>
+      <c r="L29" t="n">
+        <v>25.61366666666667</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.6141614879926387</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n"/>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>WLrbf_9</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>-0.002</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.007666666666666666</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.009504384952922171</v>
+      </c>
+      <c r="I30" t="n">
+        <v>24.937</v>
+      </c>
+      <c r="J30" t="n">
+        <v>26.417</v>
+      </c>
+      <c r="K30" t="n">
+        <v>26.383</v>
+      </c>
+      <c r="L30" t="n">
+        <v>25.91233333333333</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.8448345005581464</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n"/>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_10</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.446</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.414</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.389</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.4163333333333333</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.0285715476187996</v>
+      </c>
+      <c r="I31" t="n">
+        <v>18.542</v>
+      </c>
+      <c r="J31" t="n">
+        <v>20.4</v>
+      </c>
+      <c r="K31" t="n">
+        <v>20.707</v>
+      </c>
+      <c r="L31" t="n">
+        <v>19.883</v>
+      </c>
+      <c r="M31" t="n">
+        <v>1.17144056614068</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n"/>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_2</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.334</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.468</v>
+      </c>
+      <c r="F32" t="n">
         <v>0.249</v>
       </c>
-      <c r="E23" t="n">
-        <v>0.305</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0.178</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0.244</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0.06364746656387826</v>
-      </c>
-      <c r="I23" t="n">
-        <v>21.586</v>
-      </c>
-      <c r="J23" t="n">
-        <v>22.217</v>
-      </c>
-      <c r="K23" t="n">
-        <v>24.02</v>
-      </c>
-      <c r="L23" t="n">
-        <v>22.60766666666666</v>
-      </c>
-      <c r="M23" t="n">
-        <v>1.26315253763484</v>
+      <c r="G32" t="n">
+        <v>0.3503333333333334</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.1104098425564195</v>
+      </c>
+      <c r="I32" t="n">
+        <v>20.325</v>
+      </c>
+      <c r="J32" t="n">
+        <v>19.435</v>
+      </c>
+      <c r="K32" t="n">
+        <v>22.962</v>
+      </c>
+      <c r="L32" t="n">
+        <v>20.90733333333333</v>
+      </c>
+      <c r="M32" t="n">
+        <v>1.834193646628767</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n"/>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_3</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.522</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.381</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.4476666666666667</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.07081195755896977</v>
+      </c>
+      <c r="I33" t="n">
+        <v>18.643</v>
+      </c>
+      <c r="J33" t="n">
+        <v>18.428</v>
+      </c>
+      <c r="K33" t="n">
+        <v>20.841</v>
+      </c>
+      <c r="L33" t="n">
+        <v>19.304</v>
+      </c>
+      <c r="M33" t="n">
+        <v>1.335414916795526</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n"/>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_4</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.421</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.486</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.357</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.4213333333333333</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.06450064599159712</v>
+      </c>
+      <c r="I34" t="n">
+        <v>18.955</v>
+      </c>
+      <c r="J34" t="n">
+        <v>19.091</v>
+      </c>
+      <c r="K34" t="n">
+        <v>21.254</v>
+      </c>
+      <c r="L34" t="n">
+        <v>19.76666666666667</v>
+      </c>
+      <c r="M34" t="n">
+        <v>1.289862137336133</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n"/>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_5</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.509</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.416</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.304</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.4096666666666667</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.1026466430689934</v>
+      </c>
+      <c r="I35" t="n">
+        <v>17.461</v>
+      </c>
+      <c r="J35" t="n">
+        <v>20.361</v>
+      </c>
+      <c r="K35" t="n">
+        <v>22.098</v>
+      </c>
+      <c r="L35" t="n">
+        <v>19.97333333333333</v>
+      </c>
+      <c r="M35" t="n">
+        <v>2.342681440856468</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n"/>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_6</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.523</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.553</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.508</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.02291287847477922</v>
+      </c>
+      <c r="I36" t="n">
+        <v>17.212</v>
+      </c>
+      <c r="J36" t="n">
+        <v>17.815</v>
+      </c>
+      <c r="K36" t="n">
+        <v>18.593</v>
+      </c>
+      <c r="L36" t="n">
+        <v>17.87333333333333</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.6923455303050157</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n"/>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_7</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.504</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.5659999999999999</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.489</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.5196666666666666</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.04082074635933708</v>
+      </c>
+      <c r="I37" t="n">
+        <v>17.545</v>
+      </c>
+      <c r="J37" t="n">
+        <v>17.547</v>
+      </c>
+      <c r="K37" t="n">
+        <v>18.937</v>
+      </c>
+      <c r="L37" t="n">
+        <v>18.00966666666667</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0.8030948470344791</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n"/>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_8</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.482</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.551</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.479</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.504</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.04073082370883264</v>
+      </c>
+      <c r="I38" t="n">
+        <v>17.933</v>
+      </c>
+      <c r="J38" t="n">
+        <v>17.85</v>
+      </c>
+      <c r="K38" t="n">
+        <v>19.127</v>
+      </c>
+      <c r="L38" t="n">
+        <v>18.30333333333333</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0.7145224512451179</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n"/>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>WLsigmoidhyperbolictangent_9</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>SVR - Tanimoto Kernel</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.358</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-0.958</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-0.705</v>
+      </c>
+      <c r="G39" t="n">
+        <v>-0.4349999999999999</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.6983115350615369</v>
+      </c>
+      <c r="I39" t="n">
+        <v>19.959</v>
+      </c>
+      <c r="J39" t="n">
+        <v>37.274</v>
+      </c>
+      <c r="K39" t="n">
+        <v>34.595</v>
+      </c>
+      <c r="L39" t="n">
+        <v>30.60933333333334</v>
+      </c>
+      <c r="M39" t="n">
+        <v>9.320217826495975</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="I1:M1"/>
-    <mergeCell ref="A4:A23"/>
+    <mergeCell ref="A4:A39"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>